<commit_message>
pushing chnages for 15-02
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="76">
   <si>
     <t>TC- 101</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>Hotel select title</t>
+  </si>
+  <si>
+    <t>TC-118</t>
+  </si>
+  <si>
+    <t>Results found</t>
+  </si>
+  <si>
+    <t>1 result(s) found. Show all</t>
   </si>
 </sst>
 </file>
@@ -613,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="S19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AE32" sqref="AE32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -632,6 +641,8 @@
     <col min="13" max="13" width="32.21875" customWidth="1"/>
     <col min="14" max="14" width="26.109375" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="25" max="25" width="12.109375" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -941,7 +952,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:27">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -994,7 +1005,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:27">
       <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
@@ -1071,7 +1082,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="28.8">
+    <row r="20" spans="1:27" ht="28.8">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1148,7 +1159,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:27">
       <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
@@ -1225,7 +1236,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="28.8">
+    <row r="23" spans="1:27" ht="28.8">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -1302,7 +1313,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:27">
       <c r="A25" s="2" t="s">
         <v>64</v>
       </c>
@@ -1379,7 +1390,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="28.8">
+    <row r="26" spans="1:27" ht="28.8">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -1456,7 +1467,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="15" customHeight="1">
+    <row r="28" spans="1:27" ht="15" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>70</v>
       </c>
@@ -1503,7 +1514,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:27">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -1548,6 +1559,172 @@
       </c>
       <c r="O29" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
+      <c r="A31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA31" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" ht="28.8">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" t="s">
+        <v>28</v>
+      </c>
+      <c r="L32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M32" t="s">
+        <v>6</v>
+      </c>
+      <c r="N32" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" t="s">
+        <v>35</v>
+      </c>
+      <c r="P32" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R32" t="s">
+        <v>42</v>
+      </c>
+      <c r="S32" t="s">
+        <v>44</v>
+      </c>
+      <c r="T32" t="s">
+        <v>46</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V32" t="s">
+        <v>50</v>
+      </c>
+      <c r="W32" t="s">
+        <v>51</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>